<commit_message>
Updated test data for demo.
</commit_message>
<xml_diff>
--- a/TestData/Delegate_ValidDuplicate.xlsx
+++ b/TestData/Delegate_ValidDuplicate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neogis\D Drive\FREEDOM\Python\CloudAutomation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63ADAAFE-31CB-43D2-B88A-7C34862A4AA3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1BB0C4F-096F-4598-AAB7-B511B2B064D3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{458AF82A-ED03-4F93-994B-60962EF35F93}"/>
   </bookViews>
@@ -415,10 +415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48B209AA-B2EF-4EBA-BC33-9B6FB480ED25}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -437,31 +437,32 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
-      <c r="A3" s="3" t="s">
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{33C94BEA-23FF-47CE-8483-7FE947C6F5CA}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE1CBFDB-0592-473C-9BC6-C8164F88B115}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{33C94BEA-23FF-47CE-8483-7FE947C6F5CA}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{DC09AA2C-FBEC-4879-9447-A3904F9E4BC8}"/>
+    <hyperlink ref="A1" r:id="rId1" xr:uid="{DC09AA2C-FBEC-4879-9447-A3904F9E4BC8}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE1CBFDB-0592-473C-9BC6-C8164F88B115}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Filter PROD validation tests.
</commit_message>
<xml_diff>
--- a/TestData/Delegate_ValidDuplicate.xlsx
+++ b/TestData/Delegate_ValidDuplicate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neogis\D Drive\FREEDOM\Python\CloudAutomation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1BB0C4F-096F-4598-AAB7-B511B2B064D3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DEBFDDD-4303-4705-A974-BAC44F8F1CF1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{458AF82A-ED03-4F93-994B-60962EF35F93}"/>
   </bookViews>
@@ -418,7 +418,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Delegate test case Print addition.
</commit_message>
<xml_diff>
--- a/TestData/Delegate_ValidDuplicate.xlsx
+++ b/TestData/Delegate_ValidDuplicate.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neogis\D Drive\FREEDOM\Python\CloudAutomation\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neogis\D Drive\FREEDOM\Python\STL_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DEBFDDD-4303-4705-A974-BAC44F8F1CF1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00F90C61-8570-48FE-9B34-46B574671A4E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{458AF82A-ED03-4F93-994B-60962EF35F93}"/>
+    <workbookView xWindow="1770" yWindow="1770" windowWidth="25995" windowHeight="13095" xr2:uid="{458AF82A-ED03-4F93-994B-60962EF35F93}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>${EMAIL USER}</t>
   </si>
@@ -41,13 +41,25 @@
   </si>
   <si>
     <t>paluser_1@test.onelxk.co</t>
+  </si>
+  <si>
+    <t>${FILE PATH}</t>
+  </si>
+  <si>
+    <t>${FILE NAME}</t>
+  </si>
+  <si>
+    <t>C:\\Users\\neogis\\Downloads\\Input\\Hello.txt</t>
+  </si>
+  <si>
+    <t>Hello.txt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -68,6 +80,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color theme="1"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF808080"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -91,13 +115,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -415,26 +445,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48B209AA-B2EF-4EBA-BC33-9B6FB480ED25}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="55.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="2" width="55.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:3">
       <c r="A2" s="3" t="s">
         <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>